<commit_message>
Update metrics per 2/4 mtg discussion
</commit_message>
<xml_diff>
--- a/ProposedClicMetricTable.xlsx
+++ b/ProposedClicMetricTable.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\klgrabowski\AppData\Local\Microsoft\Windows\INetCache\Content.Outlook\RP0IK2GE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mim18\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18960" windowHeight="6130"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22296" windowHeight="8904"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,17 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="94">
   <si>
     <t>unique patients w/ age</t>
   </si>
   <si>
-    <t>unique patients w/age &gt; 120</t>
-  </si>
-  <si>
-    <t>unique patients w/age &lt; 0</t>
-  </si>
-  <si>
     <t>presentation_ref</t>
   </si>
   <si>
@@ -56,9 +50,6 @@
     <t>1/1/2020-12/31/2020</t>
   </si>
   <si>
-    <t>unique patients with administrative gender</t>
-  </si>
-  <si>
     <t>unique patients with RxNorm/NDC code</t>
   </si>
   <si>
@@ -71,9 +62,6 @@
     <t>uniq_pt_age_over_120</t>
   </si>
   <si>
-    <t>uniq_pt_age_negative</t>
-  </si>
-  <si>
     <t>uniq_pt_with_gender</t>
   </si>
   <si>
@@ -86,9 +74,6 @@
     <t>A2 numerator</t>
   </si>
   <si>
-    <t>B numerator</t>
-  </si>
-  <si>
     <t>H1 numerator</t>
   </si>
   <si>
@@ -113,9 +98,6 @@
     <t>L2 numerator</t>
   </si>
   <si>
-    <t>unique patient with insurance status</t>
-  </si>
-  <si>
     <t>L4 numerator</t>
   </si>
   <si>
@@ -131,9 +113,6 @@
     <t>unique patients with at least one opioid code from list</t>
   </si>
   <si>
-    <t>K numerator</t>
-  </si>
-  <si>
     <t>unique encounters with at least one vital sign coded</t>
   </si>
   <si>
@@ -155,9 +134,6 @@
     <t>uniq_pt_opioid</t>
   </si>
   <si>
-    <t>uniq_pt_insurance</t>
-  </si>
-  <si>
     <t>uniq_pt_vital_sign</t>
   </si>
   <si>
@@ -257,19 +233,79 @@
     <t>M1 numerator</t>
   </si>
   <si>
-    <t>unique patients with at least one clinical visit cpt code from list</t>
-  </si>
-  <si>
-    <t>unique patients with at least one clinical visit cpt code from list in time frame</t>
-  </si>
-  <si>
-    <t>M2 &amp; M3 numerator numerator</t>
-  </si>
-  <si>
     <t>uniq_pt_clin_vis_anytime</t>
   </si>
   <si>
     <t>uniq_pt_clin_vis_timeframe</t>
+  </si>
+  <si>
+    <t>variable_name</t>
+  </si>
+  <si>
+    <t>unique patients w/DOB &gt;2021</t>
+  </si>
+  <si>
+    <t>unique patients with administrative gender (excludes null, unknown, not specified)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D1 numerator </t>
+  </si>
+  <si>
+    <t xml:space="preserve">J3 </t>
+  </si>
+  <si>
+    <t>J4</t>
+  </si>
+  <si>
+    <t>L3 numerator</t>
+  </si>
+  <si>
+    <t>B1 numerator</t>
+  </si>
+  <si>
+    <t>K1 numerator</t>
+  </si>
+  <si>
+    <t>M3 numerator</t>
+  </si>
+  <si>
+    <t>unique patients with at least one clinical visit cpt code from list/encounter type</t>
+  </si>
+  <si>
+    <t>unique patients with at least one clinical visit cpt code from list/encounter type in time frame</t>
+  </si>
+  <si>
+    <t>unique encounters with RxNorm/NDC code</t>
+  </si>
+  <si>
+    <t>uniq_enc_med_rxnorm</t>
+  </si>
+  <si>
+    <t>uniq_pt_insurance_value_set</t>
+  </si>
+  <si>
+    <t>uniq_pt_any_insurance_value</t>
+  </si>
+  <si>
+    <t>NOT A SCRIPT VALUE</t>
+  </si>
+  <si>
+    <t>M2 &amp; M3 numerator</t>
+  </si>
+  <si>
+    <t>OMIT THIS unique patients with at least one clinical visit cpt code from list/encounter type in time frame</t>
+  </si>
+  <si>
+    <t>uniq_pt_birthdate_in_future</t>
+  </si>
+  <si>
+    <t>unique patients w/age DOD - DOB &gt; 120 OR if no DOD, 12/31/2020 - DOB &gt; 120</t>
+  </si>
+  <si>
+    <t>unique patients with any non null insurance provider</t>
+  </si>
+  <si>
+    <t>unique patient with insurance provider harmonized to a CDM value set</t>
   </si>
 </sst>
 </file>
@@ -286,18 +322,35 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -312,13 +365,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -599,326 +660,437 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B6:B7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.6328125" customWidth="1"/>
-    <col min="2" max="2" width="29" style="2" customWidth="1"/>
-    <col min="3" max="3" width="51.36328125" customWidth="1"/>
-    <col min="4" max="4" width="20.6328125" customWidth="1"/>
+    <col min="1" max="1" width="16.5546875" customWidth="1"/>
+    <col min="2" max="2" width="93.88671875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" customWidth="1"/>
+    <col min="4" max="4" width="20.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D1" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
       </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B6" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B7" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>78</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="B18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C9" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>67</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>60</v>
-      </c>
-      <c r="B11" t="s">
-        <v>62</v>
-      </c>
-      <c r="C11" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>61</v>
-      </c>
-      <c r="B12" t="s">
-        <v>63</v>
-      </c>
-      <c r="C12" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>54</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="C22" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>31</v>
       </c>
-      <c r="C13" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>53</v>
-      </c>
-      <c r="B14" t="s">
-        <v>55</v>
-      </c>
-      <c r="C14" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>51</v>
-      </c>
-      <c r="B15" t="s">
-        <v>65</v>
-      </c>
-      <c r="C15" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>52</v>
-      </c>
-      <c r="B16" t="s">
-        <v>64</v>
-      </c>
-      <c r="C16" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="B23" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C17" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>47</v>
-      </c>
-      <c r="B18" t="s">
-        <v>48</v>
-      </c>
-      <c r="C18" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>68</v>
-      </c>
-      <c r="B19" t="s">
-        <v>31</v>
-      </c>
-      <c r="C19" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>69</v>
-      </c>
-      <c r="B20" t="s">
-        <v>55</v>
-      </c>
-      <c r="C20" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>37</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C21" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+      <c r="C23" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>35</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C23" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>27</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C24" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>28</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C25" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C24" s="5"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C25" s="5"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>30</v>
+        <v>79</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C26" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="C26" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>76</v>
+        <v>22</v>
       </c>
       <c r="B27" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>77</v>
       </c>
-      <c r="C27" t="s">
+      <c r="B29" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>24</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>68</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>88</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+    </row>
+    <row r="33" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="5" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>79</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C28" t="s">
-        <v>81</v>
+      <c r="B33" s="6" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>